<commit_message>
Versión final del artículo RPSP
</commit_message>
<xml_diff>
--- a/Paper_resultados/Cox_model/Output/Multivariate_model/Multivariate_models.xlsx
+++ b/Paper_resultados/Cox_model/Output/Multivariate_model/Multivariate_models.xlsx
@@ -387,39 +387,39 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Group_age[65,Inf]</t>
+          <t>sexMale</t>
         </is>
       </c>
       <c r="B2">
-        <v>2.205097593664796</v>
+        <v>1.085687007161959</v>
       </c>
       <c r="C2">
-        <v>1.851078123733235</v>
+        <v>0.9164260556025183</v>
       </c>
       <c r="D2">
-        <v>2.626823436160396</v>
+        <v>1.286209913297725</v>
       </c>
       <c r="E2">
-        <v>8.271226470156217e-019</v>
+        <v>0.3417468030667726</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CCInon-CCI</t>
+          <t>age</t>
         </is>
       </c>
       <c r="B3">
-        <v>4.689739723813502</v>
+        <v>1.034481121476051</v>
       </c>
       <c r="C3">
-        <v>3.622798087667819</v>
+        <v>1.027853885834152</v>
       </c>
       <c r="D3">
-        <v>6.070903800016297</v>
+        <v>1.041151087172152</v>
       </c>
       <c r="E3">
-        <v>8.540211709376492e-032</v>
+        <v>4.73606371603818e-25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>